<commit_message>
small changes about menu report
</commit_message>
<xml_diff>
--- a/WebUI/Files/Templates/Repair/Списание.xlsx
+++ b/WebUI/Files/Templates/Repair/Списание.xlsx
@@ -52,9 +52,6 @@
     <t>Вид заявки</t>
   </si>
   <si>
-    <t>Заправка оборудования</t>
-  </si>
-  <si>
     <t>Период выборки данных</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>Автор заявки</t>
+  </si>
+  <si>
+    <t>Ремонт оборудования</t>
   </si>
 </sst>
 </file>
@@ -749,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +770,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -806,7 +806,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="I3" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="24"/>
     </row>
@@ -822,7 +822,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="I4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" s="4">
         <f>'!Data'!B1</f>
@@ -834,14 +834,14 @@
         <v>9</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C5" s="22"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="I5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" s="6">
         <f>'!Data'!E1</f>
@@ -856,16 +856,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="D7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="E7" s="17" t="s">
         <v>17</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>18</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>0</v>
@@ -880,7 +880,7 @@
         <v>3</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>